<commit_message>
remove and add diff project
</commit_message>
<xml_diff>
--- a/critical_classification/dashcam_video/metadata.xlsx
+++ b/critical_classification/dashcam_video/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khoavo2003/PycharmProjects/DAAD-RISE-Germany/critical_classification/dashcam_video/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D22BAEF-D3B9-654B-8547-34C387F5F19D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F71653-A35B-5F4F-AE2B-FF87BC596D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="79">
   <si>
     <t>path</t>
   </si>
@@ -28,55 +28,235 @@
     <t>critical_driving_time</t>
   </si>
   <si>
+    <t>train_or_test</t>
+  </si>
+  <si>
     <t>Vollbremsungen Überholen durchs Bankett und Schleicherei  DDG Dashcam Germany  580.mp4</t>
   </si>
   <si>
+    <t>0:14-0:15, 0:34-0:35, 0:50-0:51, 1:27-1:28, 1:37-1:38, 1:56-1:57, 2:25-2:26</t>
+  </si>
+  <si>
+    <t>train</t>
+  </si>
+  <si>
     <t>Mega-Close-Call Instant-Karma und gefährliches Überholen  DDG Dashcam Germany  579.mp4</t>
   </si>
   <si>
+    <t>0:15-0:17, 5:45-5:47, 7:10-7:12, 7:45-7:46</t>
+  </si>
+  <si>
     <t>Dämlichste Ampel des Jahres blind überholen und Feuerwehr blockiert  DDG Dashcam Germany  578.mp4</t>
   </si>
   <si>
+    <t>4:34-4:35, 4:50-4:51, 5:15-5:16, 9:26-9:27</t>
+  </si>
+  <si>
     <t>Völlig unlogisches Road-Rage Rote Ampeln und Kreuzungs-Chaos  DDG Dashcam Germany  577.mp4</t>
   </si>
   <si>
+    <t>4:04-4:05, 4:19-4:20, 4:39-4:40, 7:28-7:31</t>
+  </si>
+  <si>
     <t>LKW in Engstelle blockiert Missgeschick in der Abfahrt und Überholen  DDG Dashcam Germany  576.mp4</t>
   </si>
   <si>
+    <t>1:07-1:08, 1:48-1:50, 2:13-2:14, 4:27-4:28, 4:43-4:44</t>
+  </si>
+  <si>
     <t>Hund verursacht Unfall verrückte Überholmanöver und Sicherheitsabstand  DDG Dashcam Germany  575.mp4</t>
   </si>
   <si>
+    <t>0:16-0:17, 0:43-0:44, 1:54-1:55, 2:34-2:35, 3:33-3:34, 7:12-7:14</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
     <t>LKW übersehen Vollbremsungen und 2 kaputte Reifen  DDG Dashcam Germany  574.mp4</t>
   </si>
   <si>
-    <t>0:15-0:17, 5:45-5:47, 7:10-7:12, 7:45-7:46</t>
-  </si>
-  <si>
-    <t>4:34-4:35, 4:50-4:51, 5:15-5:16, 9:26-9:27</t>
-  </si>
-  <si>
-    <t>4:04-4:05, 4:19-4:20, 4:39-4:40, 7:28-7:31</t>
-  </si>
-  <si>
-    <t>1:07-1:08, 1:48-1:50, 2:13-2:14, 4:27-4:28, 4:43-4:44</t>
-  </si>
-  <si>
-    <t>0:16-0:17, 0:43-0:44, 1:54-1:55, 2:34-2:35, 3:33-3:34, 7:12-7:14</t>
-  </si>
-  <si>
     <t>0:18-0:19, 1:28-1:29, 3:37-3:38, 4:56-4:57</t>
   </si>
   <si>
-    <t>train_or_test</t>
-  </si>
-  <si>
-    <t>train</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>0:14-0:15, 0:34-0:35, 0:50-0:51, 1:27-1:28, 1:37-1:38, 1:56-1:57, 2:25-2:26</t>
+    <t>Gefährliches Überholen Stress an Engstelle und offene Auto-Tür  DDG Dashcam Germany  573.mp4</t>
+  </si>
+  <si>
+    <t>Abfahrt im letzten Moment Rote Ampeln und Vordrängeln  DDG Dashcam Germany  572.mp4</t>
+  </si>
+  <si>
+    <t>190kmh-Unfall Einsatzfahrten gehen schief und rote Ampeln  DDG Dashcam Germany  Unfallfolge 11.mp4</t>
+  </si>
+  <si>
+    <t>Abdrängen merkwürdiges Überholen und Ziegen   DDG Dashcam Germany  571.mp4</t>
+  </si>
+  <si>
+    <t>Polizei-Karma unglaubliche Ladungssicherung und blind überholen  DDG Dashcam Germany  570.mp4</t>
+  </si>
+  <si>
+    <t>Vollbremsung bei Schnee Close-Call auf Landstraße und blind losfahren  DDG Dashcam Germany  569.mp4</t>
+  </si>
+  <si>
+    <t>Überholer Ampeln und Sommerreifen bei Schnee  Best-Of-Batimus .mp4</t>
+  </si>
+  <si>
+    <t>Unangenehmste Blockade des Jahres Nötigung und auf Aspahlt festgefahrn  DDG Dashcam Germany  568.mp4</t>
+  </si>
+  <si>
+    <t>Unglaublicher Überholer Vorfahrt nehmen und Close-Call an Auffahrt  DDG Dashcam Germany  567.mp4</t>
+  </si>
+  <si>
+    <t>Vollbremsungen mit Kinderwagen bei Rot auf die Kreuzung und Überholen  DDG Dashcam Germany  566.mp4</t>
+  </si>
+  <si>
+    <t>200kmh-Vollbremsung kein Schulterblick und Close-Call  DDG Dashcam Germany  564.mp4</t>
+  </si>
+  <si>
+    <t>Tür kaputt getreten und Mega-Close-Call  DDG Dashcam Germany  565  wwwdashcam-shopcom.mp4</t>
+  </si>
+  <si>
+    <t>Rettungsgasse blockiert verwirrt in Baustelle und gefährlich Überholen  DDG Dashcam Germany  563.mp4</t>
+  </si>
+  <si>
+    <t>Blind überholen und kein Schulterblick  DDG Dashcam Germany  562  wwwdashcam-shopcom.mp4</t>
+  </si>
+  <si>
+    <t>Kein Schulterblick Vollbremsung und Chaos in der Stadt  DDG Dashcam Germany  561.mp4</t>
+  </si>
+  <si>
+    <t>Einsatzfahrzeug an Ampel blockiert + blind überholt DDG Dashcam Germany 560 wwwdashcam-shopcom.mp4</t>
+  </si>
+  <si>
+    <t>Falsche Schuldzuweisung bei Unfall und Überholen  DDG Dashcam Germany  559   wwwdashcam-shopcom.mp4</t>
+  </si>
+  <si>
+    <t>Völlig unnötige Fahrerflucht!  DDG Dashcam Germany .mp4</t>
+  </si>
+  <si>
+    <t>Vorfahrt nehmen Engstellen-Chaos und Motorrad vs Autofahrer  DDG Dashcam Germany  558.mp4</t>
+  </si>
+  <si>
+    <t>Steinschlag auf der Autobahn Auto vs Radfahrer und Vorfahrt nehmen  DDG Dashcam Germany  557.mp4</t>
+  </si>
+  <si>
+    <t>Überholmanöver des Jahres Sekundenschlaf und Autobahn-Auffahrt  DDG Dashcam Germany  556.mp4</t>
+  </si>
+  <si>
+    <t>Plötzliches Glatteis Vorfahrt nehmen und Ausweichen  DDG Dashcam Germany  555.mp4</t>
+  </si>
+  <si>
+    <t>Egoismus in Engstellen Vorfahrt nehmen und Abfahrt fällt vom Himmel  DDG Dashcam Germany  554.mp4</t>
+  </si>
+  <si>
+    <t>Überholen bei Gegenverkehr erzwungene Spurwechsel und Abbiege-Fail  DDG Dashcam Germany  553.mp4</t>
+  </si>
+  <si>
+    <t>Polizei wird blockiert Stress auf der Autobahn und engste Autobrücke   DDG Dashcam Germany  552.mp4</t>
+  </si>
+  <si>
+    <t>Road-Rage Mutter des Jahres und sinnloses Überholen  DDG Dashcam Germany  551.mp4</t>
+  </si>
+  <si>
+    <t>LKW ausgebremst Panne auf der Autobahn und Ungeduld  DDG Dashcam Germany  550.mp4</t>
+  </si>
+  <si>
+    <t>Betrug im Parkhaus Vollbremsung für Reh und Engstellen-Chaos  DDG Dashcam Germany  549.mp4</t>
+  </si>
+  <si>
+    <t>Leitplanke plattgefahren Vollbremsung direkt vorm LKW und Überholen   DDG Dashcam Germany  548.mp4</t>
+  </si>
+  <si>
+    <t>Ausbremsen auf der Landstraße Straße blockieren und LKW-Überholmanöver  DDG Dashcam Germany  547.mp4</t>
+  </si>
+  <si>
+    <t>Dreistigkeit an Engstellen Kurven schneiden und Road-Rage  DDG Dashcam Germany  546.mp4</t>
+  </si>
+  <si>
+    <t>Festgefahren im Schnee Stress in der Engstelle und Überholmanöver  DDG Dashcam Germany  545.mp4</t>
+  </si>
+  <si>
+    <t>Best-Of Dashcam 2023 - Unfälle  Road-Rage Vollbremsungen und  Nötigungen  DDG Dashcam Germany .mp4</t>
+  </si>
+  <si>
+    <t>Überholen Kontrollverlust und rote Ampeln  DDG Dashcam Germany 544.mp4</t>
+  </si>
+  <si>
+    <t>Motorrad übersehen keine Rettungsgasse und unnötiger Unfall   DDG Dashcam Germany  543.mp4</t>
+  </si>
+  <si>
+    <t>Vollbremsungen Spiegel abgefahren und Handy am Steuer  DDG Dashcam Germany  542.mp4</t>
+  </si>
+  <si>
+    <t>Kein Schulterblick Road-Rage und merkwürdige Fahrweise  DDG Dashcam Germany  541.mp4</t>
+  </si>
+  <si>
+    <t>Schlimmstes Parkmanöver des Jahres Vorfahrt nehmen und Vollbremsungen  DDG Dashcam Germany  540.mp4</t>
+  </si>
+  <si>
+    <t>Road-Rage über den Bordstein fahren und Taxi-Notfall  DDG Dashcam Germany  539.mp4</t>
+  </si>
+  <si>
+    <t>Kuh rennt vors Auto blind rückwärts fahren und Abfahrt kurz vor knapp  DDG Dashcam Germany  538.mp4</t>
+  </si>
+  <si>
+    <t>LKW verliert Ladung  Close Calls und intelligentes Überholen  DDG Dashcam Germany  537.mp4</t>
+  </si>
+  <si>
+    <t>Bahnübergang blockiert Ampel-Unfall und Schulterblick  DDG Dashcam Germany  536.mp4</t>
+  </si>
+  <si>
+    <t>Eltern des Jahres absurdes Überholen und blind fahren  DDG Dashcam Germany  535.mp4</t>
+  </si>
+  <si>
+    <t>0:24-0:25, 2:04-2:06,  2:43-2:44, 4:43-4:45, 5:19-5:20, 5:31-5:32, 6:43-6:44</t>
+  </si>
+  <si>
+    <t>1:12-1:13, 1:51-1:52, 2:31-2:32, 3:18-3:19, 3:32-3:33, 4:18-4:19, 5:09-5:10, 5:18-5:19, 7:20-7:21</t>
+  </si>
+  <si>
+    <t>0:14-0:15, 3:08-3:09</t>
+  </si>
+  <si>
+    <t>3:20-3:21, 3:51-3:52, 4:03-4:04, 4:26-4:27, 4:51-4:53, 5:29-5:31, 6:37-6:38</t>
+  </si>
+  <si>
+    <t>1:09-1:10, 1:47-1:48, 5:07-5:08, 5:29-5:30, 5:55-5:56, 7:31-7:32</t>
+  </si>
+  <si>
+    <t>0:15-0:16, 0:46-0:47, 1:12-1:13, 2:44-2:48, 3:05-3:06, 3:38-3:39, 4:42-4:43, 4:44-4:45, 6:40-6:41, 7:35-7:36, 8:11-8:12, 8:39-8:40, 9:01-9:02</t>
+  </si>
+  <si>
+    <t>1:14-1:15, 3:23:3:24, 5:45-5:47, 7:58-7:59, 9:48-9:52, 10:01-10:02, 10:53-10:54, 11:50-11:51, 12:47-12:48</t>
+  </si>
+  <si>
+    <t>0:57-1:00, 1:23-1:24, 2:53-2:55, 4:12-4:14, 7:48-7:53</t>
+  </si>
+  <si>
+    <t>0:28-0:29, 1:27-1:28, 4:04-4:05, 8:21-8:22</t>
+  </si>
+  <si>
+    <t>0:32-0:34, 0:42-0:44, 0:57-0:58, 1:51-1:53, 2:49-2:50, 3:15-3:17, 5:09-5:11, 6:52-6:53, 7:03-7:05</t>
+  </si>
+  <si>
+    <t>0:45-0:47, 3:15-3:17, 3:26-3:28, 4:48-4:49, 5:11-5:12, 6:16-6:17, 6:57-6:58</t>
+  </si>
+  <si>
+    <t>1:27-1:28, 1:40-1:41, 2:17-2:19, 3:23-3:25, 4:00-4:02, 8:13-8:14, 8:27-8:28</t>
+  </si>
+  <si>
+    <t>0:21-0:23, 6:05-6:06, 6:58-6:59, 7:14-7:16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2:03-2:04, 2:32-2:34, 3:19-3:20, 3:48-3:49, 4:54-4:56, 5:19-5:21, 6:14-6:15, 7:36-7:39, </t>
+  </si>
+  <si>
+    <t>0:14-0:15, 0:45-0:47, 1:11-1:14, 3:58-4:00, 5:04-5:05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0:02-0:03, 0:25-0:26, 3:42-3:43, 3:53-3:54, 4:04-4:05, 6:27-6:30, </t>
+  </si>
+  <si>
+    <t>0:02-0:03, 0:37-0:39, 2:49-2:50, 4:29-4:31, 5:28-5:29</t>
   </si>
 </sst>
 </file>
@@ -440,16 +620,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="85.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="87.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="105.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -459,85 +639,402 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>15</v>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>